<commit_message>
updated time card and weekly report
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ranson_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ranson_TimeCard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranson_kr\source\repos\Yellow Project\YellowLib\YellowLib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranson_kr\Source\Repos\Yellow Project\YellowLib\YellowLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="19">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -635,8 +635,8 @@
   </sheetPr>
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -710,11 +710,11 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>0</v>
+        <v>2.4999999999999964</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>0</v>
+        <v>2.4999999999999964</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
@@ -742,11 +742,11 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
+      <c r="B8" s="4">
+        <v>43504</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.70833333333333337</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>14</v>
@@ -754,20 +754,20 @@
       <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>16</v>
+      <c r="F8" s="6">
+        <v>0.72916666666666663</v>
       </c>
       <c r="G8" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>0.49999999999999822</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>13</v>
+      <c r="B9" s="4">
+        <v>43506</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>14</v>
@@ -775,12 +775,12 @@
       <c r="E9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>16</v>
+      <c r="F9" s="6">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G9" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>1.9999999999999982</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Undated weekly reports and timecard
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ranson_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ranson_TimeCard.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranson_kr\Source\Repos\Yellow Project\YellowLib\YellowLib\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Time Sheet'!$7:$7</definedName>
     <definedName name="WorkweekHours">'Time Sheet'!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="24">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -94,12 +89,27 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>6:00PM</t>
+  </si>
+  <si>
+    <t>8:15PM</t>
+  </si>
+  <si>
+    <t>7:30PM</t>
+  </si>
+  <si>
+    <t>3:45PM</t>
+  </si>
+  <si>
+    <t>4:00PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
@@ -621,7 +631,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -635,21 +645,21 @@
   </sheetPr>
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="3" max="5" width="20.7265625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" customWidth="1"/>
+    <col min="8" max="8" width="2.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
@@ -710,18 +720,18 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>2.4999999999999964</v>
+        <v>6.4999999999999964</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>2.4999999999999964</v>
+        <v>6.4999999999999964</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
@@ -741,7 +751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>43504</v>
       </c>
@@ -762,7 +772,7 @@
         <v>0.49999999999999822</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>43506</v>
       </c>
@@ -783,12 +793,12 @@
         <v>1.9999999999999982</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>18</v>
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>43508</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>14</v>
@@ -797,19 +807,18 @@
         <v>15</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G10" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>43515</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>14</v>
@@ -818,19 +827,18 @@
         <v>15</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G11" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>18</v>
+      <c r="B12" s="4">
+        <v>43516</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>14</v>
@@ -839,14 +847,13 @@
         <v>15</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G12" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
@@ -867,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
@@ -888,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
@@ -909,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
@@ -951,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
@@ -972,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
@@ -993,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
@@ -1014,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
@@ -1056,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1077,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1119,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1140,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="4" t="s">
         <v>18</v>
       </c>
@@ -1161,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
         <v>18</v>
       </c>
@@ -1182,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>18</v>
       </c>
@@ -1203,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
@@ -1224,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
         <v>18</v>
       </c>
@@ -1245,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="4" t="s">
         <v>18</v>
       </c>
@@ -1266,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="4" t="s">
         <v>18</v>
       </c>
@@ -1287,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
         <v>18</v>
       </c>
@@ -1308,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
         <v>18</v>
       </c>
@@ -1329,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="4" t="s">
         <v>18</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
added time to timecard
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ranson_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ranson_TimeCard.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranson_kr\Source\Repos\Yellow Project\YellowLib\YellowLib\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Time Sheet'!$7:$7</definedName>
     <definedName name="WorkweekHours">'Time Sheet'!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
@@ -631,7 +636,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -649,17 +654,17 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" customWidth="1"/>
-    <col min="3" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" customWidth="1"/>
-    <col min="8" max="8" width="2.7265625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
@@ -731,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
@@ -751,7 +756,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>43504</v>
       </c>
@@ -772,7 +777,7 @@
         <v>0.49999999999999822</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>43506</v>
       </c>
@@ -793,7 +798,7 @@
         <v>1.9999999999999982</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>43508</v>
       </c>
@@ -813,7 +818,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>43515</v>
       </c>
@@ -853,7 +858,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
@@ -874,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
@@ -895,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
@@ -916,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
@@ -958,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
@@ -979,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
@@ -1000,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
@@ -1021,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
@@ -1063,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1084,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1105,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1147,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>18</v>
       </c>
@@ -1168,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>18</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>18</v>
       </c>
@@ -1210,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
@@ -1231,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>18</v>
       </c>
@@ -1252,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>18</v>
       </c>
@@ -1273,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>18</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>18</v>
       </c>
@@ -1315,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>18</v>
       </c>
@@ -1336,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>18</v>
       </c>
@@ -1357,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Updated timecard, and weekly reports
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ranson_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ranson_TimeCard.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranson_kr\Source\Repos\Yellow Project\YellowLib\YellowLib\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Time Sheet'!$7:$7</definedName>
     <definedName name="WorkweekHours">'Time Sheet'!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="30">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -119,12 +124,15 @@
   </si>
   <si>
     <t>4:30PM</t>
+  </si>
+  <si>
+    <t>5:00P&lt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
@@ -646,7 +654,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -661,20 +669,20 @@
   <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" customWidth="1"/>
-    <col min="3" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" customWidth="1"/>
-    <col min="8" max="8" width="2.7265625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
@@ -746,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
@@ -766,7 +774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>43504</v>
       </c>
@@ -787,7 +795,7 @@
         <v>0.49999999999999822</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>43506</v>
       </c>
@@ -808,7 +816,7 @@
         <v>1.9999999999999982</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>43508</v>
       </c>
@@ -828,7 +836,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>43515</v>
       </c>
@@ -868,7 +876,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>43520</v>
       </c>
@@ -888,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>43522</v>
       </c>
@@ -908,7 +916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>43523</v>
       </c>
@@ -928,7 +936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>43523</v>
       </c>
@@ -949,11 +957,11 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>18</v>
+      <c r="B17" s="4">
+        <v>43527</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>14</v>
@@ -962,14 +970,13 @@
         <v>15</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G17" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
@@ -990,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
@@ -1011,7 +1018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
@@ -1032,7 +1039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
@@ -1074,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1095,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1116,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1137,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1158,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>18</v>
       </c>
@@ -1179,7 +1186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>18</v>
       </c>
@@ -1200,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>18</v>
       </c>
@@ -1221,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
@@ -1242,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>18</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>18</v>
       </c>
@@ -1284,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>18</v>
       </c>
@@ -1305,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>18</v>
       </c>
@@ -1326,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>18</v>
       </c>
@@ -1347,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>18</v>
       </c>
@@ -1368,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Fixed formula issue in excel timecard
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ranson_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ranson_TimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="31">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -97,18 +97,6 @@
   </si>
   <si>
     <t>6:00PM</t>
-  </si>
-  <si>
-    <t>8:15PM</t>
-  </si>
-  <si>
-    <t>7:30PM</t>
-  </si>
-  <si>
-    <t>3:45PM</t>
-  </si>
-  <si>
-    <t>4:00PM</t>
   </si>
   <si>
     <t>2:00PM</t>
@@ -393,8 +381,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G12" totalsRowShown="0">
-  <autoFilter ref="B7:G12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G30" totalsRowShown="0">
+  <autoFilter ref="B7:G30"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -681,10 +669,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H37"/>
+  <dimension ref="B1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -758,11 +746,11 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>6.4999999999999964</v>
+        <v>25.999999999999993</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>6.4999999999999964</v>
+        <v>25.999999999999993</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
@@ -835,8 +823,8 @@
       <c r="B10" s="4">
         <v>43508</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>19</v>
+      <c r="C10" s="6">
+        <v>0.75</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>14</v>
@@ -844,10 +832,11 @@
       <c r="E10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>20</v>
+      <c r="F10" s="6">
+        <v>0.84375</v>
       </c>
       <c r="G10" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>2.25</v>
       </c>
     </row>
@@ -855,8 +844,8 @@
       <c r="B11" s="4">
         <v>43515</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>19</v>
+      <c r="C11" s="6">
+        <v>0.75</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>14</v>
@@ -864,19 +853,20 @@
       <c r="E11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>21</v>
+      <c r="F11" s="6">
+        <v>0.8125</v>
       </c>
       <c r="G11" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>43516</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>22</v>
+      <c r="C12" s="6">
+        <v>0.65625</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>14</v>
@@ -884,19 +874,20 @@
       <c r="E12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>23</v>
+      <c r="F12" s="6">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G12" s="5">
-        <v>0.25</v>
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>43520</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>24</v>
+      <c r="C13" s="6">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>14</v>
@@ -904,19 +895,20 @@
       <c r="E13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>23</v>
+      <c r="F13" s="6">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G13" s="5">
-        <v>2</v>
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>1.9999999999999982</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>43522</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>19</v>
+      <c r="C14" s="6">
+        <v>0.75</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>14</v>
@@ -924,8 +916,8 @@
       <c r="E14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>25</v>
+      <c r="F14" s="6">
+        <v>0.83333333333333337</v>
       </c>
       <c r="G14" s="5">
         <v>2</v>
@@ -936,7 +928,7 @@
         <v>43523</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>14</v>
@@ -945,7 +937,7 @@
         <v>15</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G15" s="5">
         <v>5</v>
@@ -956,7 +948,7 @@
         <v>43523</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>14</v>
@@ -965,18 +957,18 @@
         <v>15</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G16" s="5">
         <v>3.5</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>43527</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>14</v>
@@ -985,7 +977,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G17" s="5">
         <v>3</v>
@@ -1005,7 +997,7 @@
         <v>15</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G18" s="5">
         <v>3</v>
@@ -1016,16 +1008,16 @@
         <v>43531</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G19" s="5">
         <v>1</v>
@@ -1048,7 +1040,6 @@
         <v>16</v>
       </c>
       <c r="G20" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1069,11 +1060,10 @@
         <v>16</v>
       </c>
       <c r="G21" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>18</v>
       </c>
@@ -1090,7 +1080,6 @@
         <v>16</v>
       </c>
       <c r="G22" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1111,7 +1100,6 @@
         <v>16</v>
       </c>
       <c r="G23" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1132,7 +1120,6 @@
         <v>16</v>
       </c>
       <c r="G24" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1153,7 +1140,6 @@
         <v>16</v>
       </c>
       <c r="G25" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1174,11 +1160,10 @@
         <v>16</v>
       </c>
       <c r="G26" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>18</v>
       </c>
@@ -1195,7 +1180,6 @@
         <v>16</v>
       </c>
       <c r="G27" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1216,7 +1200,6 @@
         <v>16</v>
       </c>
       <c r="G28" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1237,7 +1220,6 @@
         <v>16</v>
       </c>
       <c r="G29" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1258,7 +1240,6 @@
         <v>16</v>
       </c>
       <c r="G30" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1283,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>18</v>
       </c>
@@ -1304,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>18</v>
       </c>
@@ -1388,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>18</v>
       </c>
@@ -1405,6 +1386,237 @@
         <v>16</v>
       </c>
       <c r="G37" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updated reports and timecard
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ranson_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ranson_TimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="36">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>3:00Pm</t>
+  </si>
+  <si>
+    <t>4:00pm</t>
+  </si>
+  <si>
+    <t>6:00pm</t>
+  </si>
+  <si>
+    <t>8:30pm</t>
+  </si>
+  <si>
+    <t>7:30PM</t>
   </si>
 </sst>
 </file>
@@ -674,8 +686,8 @@
   </sheetPr>
   <dimension ref="B1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -749,11 +761,11 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>28.999999999999993</v>
+        <v>34.999999999999993</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>28.999999999999993</v>
+        <v>34.999999999999993</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
@@ -1067,11 +1079,11 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>13</v>
+      <c r="B22" s="4">
+        <v>43548</v>
+      </c>
+      <c r="C22" s="6">
+        <v>2</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>14</v>
@@ -1080,18 +1092,18 @@
         <v>15</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>18</v>
+      <c r="B23" s="4">
+        <v>43552</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>14</v>
@@ -1100,18 +1112,18 @@
         <v>15</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G23" s="5">
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>18</v>
+      <c r="B24" s="4">
+        <v>43557</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>14</v>
@@ -1120,10 +1132,10 @@
         <v>15</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="G24" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated weekly report and time card
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ranson_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ranson_TimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="39">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>4:00PM</t>
+  </si>
+  <si>
+    <t>11:00AM</t>
   </si>
 </sst>
 </file>
@@ -692,8 +695,8 @@
   </sheetPr>
   <dimension ref="B1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -767,7 +770,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>40.999999999999993</v>
+        <v>45.999999999999993</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -775,7 +778,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>0.99999999999999289</v>
+        <v>5.9999999999999929</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1205,11 +1208,11 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>18</v>
+      <c r="B28" s="4">
+        <v>43569</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>14</v>
@@ -1218,18 +1221,18 @@
         <v>15</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="G28" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>18</v>
+      <c r="B29" s="4">
+        <v>43571</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>14</v>
@@ -1238,18 +1241,18 @@
         <v>15</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G29" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>18</v>
+      <c r="B30" s="4">
+        <v>43573</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>14</v>
@@ -1258,10 +1261,10 @@
         <v>15</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated time sheet and weekly report
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ranson_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ranson_TimeCard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranson_kr\Source\Repos\Yellow Project5\YellowLib\YellowLib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranson_kr\Source\Repos\Yellow Project\YellowLib\YellowLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="39">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -405,8 +405,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G30" totalsRowShown="0">
-  <autoFilter ref="B7:G30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G33" totalsRowShown="0">
+  <autoFilter ref="B7:G33"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -695,8 +695,8 @@
   </sheetPr>
   <dimension ref="B1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -770,7 +770,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>45.999999999999993</v>
+        <v>51.999999999999993</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -778,7 +778,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>5.9999999999999929</v>
+        <v>11.999999999999993</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1268,11 +1268,11 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>18</v>
+      <c r="B31" s="4">
+        <v>43576</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>14</v>
@@ -1281,19 +1281,18 @@
         <v>15</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G31" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>18</v>
+      <c r="B32" s="4">
+        <v>43578</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>14</v>
@@ -1302,19 +1301,18 @@
         <v>15</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G32" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
-        <v>18</v>
+      <c r="B33" s="4">
+        <v>43585</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>14</v>
@@ -1323,11 +1321,10 @@
         <v>15</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G33" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>